<commit_message>
Updated results with BIC' for benchmark models
</commit_message>
<xml_diff>
--- a/results/BIC.xlsx
+++ b/results/BIC.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Documents\Projects\SERICS Errors\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\IdeaProjects\error-analysis-updated\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F469DDE-BF50-4DE6-8CF4-893AFB1C9DEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFAA482A-BB90-4E86-B830-7D9A028A78CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{85E0CB34-C0A8-4698-AB87-F082139B7D43}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
   <si>
     <t>Midterm 1 - HW3-4</t>
   </si>
@@ -44,12 +44,6 @@
     <t>Midterm 2 - HW3-8</t>
   </si>
   <si>
-    <t>error count</t>
-  </si>
-  <si>
-    <t>jadud</t>
-  </si>
-  <si>
     <t>RED</t>
   </si>
   <si>
@@ -87,12 +81,27 @@
   </si>
   <si>
     <t>BIC'</t>
+  </si>
+  <si>
+    <t>EC</t>
+  </si>
+  <si>
+    <t>EQ</t>
+  </si>
+  <si>
+    <t>Benchmark</t>
+  </si>
+  <si>
+    <t>grades</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -156,7 +165,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -245,7 +254,7 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top/>
@@ -255,16 +264,24 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
       <right style="medium">
         <color rgb="FF000000"/>
       </right>
@@ -276,12 +293,27 @@
     </border>
     <border>
       <left style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
       <right/>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -289,17 +321,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -316,18 +344,23 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="2" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="171" fontId="2" fillId="3" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -642,414 +675,485 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1285FD72-DB01-416F-8CC2-B90C5DB835E4}">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="10.5703125" customWidth="1"/>
+    <col min="8" max="8" width="10.85546875" customWidth="1"/>
+    <col min="9" max="9" width="12.28515625" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
+    <col min="15" max="15" width="11.140625" customWidth="1"/>
+    <col min="16" max="16" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="14" t="s">
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
     </row>
-    <row r="2" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="18"/>
+      <c r="E2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="18"/>
+      <c r="G2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="17"/>
-      <c r="E2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="17"/>
-      <c r="G2" s="17" t="s">
-        <v>4</v>
-      </c>
       <c r="H2" s="18"/>
-      <c r="I2" s="19" t="s">
+      <c r="I2" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="18"/>
+      <c r="L2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="18"/>
+      <c r="N2" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="N2" s="17"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="19" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="L3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="M3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="N3" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O3" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="P3" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="C4" s="3">
+        <v>280</v>
+      </c>
+      <c r="D4" s="3">
+        <v>280</v>
+      </c>
+      <c r="E4" s="3">
+        <v>280</v>
+      </c>
+      <c r="F4" s="3">
+        <v>280</v>
+      </c>
+      <c r="G4" s="3">
+        <v>280</v>
+      </c>
+      <c r="H4" s="4">
+        <v>280</v>
+      </c>
+      <c r="I4" s="4">
+        <v>280</v>
+      </c>
+      <c r="J4" s="3">
+        <v>280</v>
+      </c>
+      <c r="K4" s="3">
+        <v>280</v>
+      </c>
+      <c r="L4" s="3">
+        <v>280</v>
+      </c>
+      <c r="M4" s="3">
+        <v>280</v>
+      </c>
+      <c r="N4" s="3">
+        <v>280</v>
+      </c>
+      <c r="O4" s="3">
+        <v>280</v>
+      </c>
+      <c r="P4" s="3">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="F5" s="3">
+        <v>0.185</v>
+      </c>
+      <c r="G5" s="3">
+        <v>0.105</v>
+      </c>
+      <c r="H5" s="4">
+        <v>0.114</v>
+      </c>
+      <c r="I5" s="4">
+        <v>0.247</v>
+      </c>
+      <c r="J5" s="3">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="N5" s="3">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="O5" s="3">
+        <v>0.19</v>
+      </c>
+      <c r="P5" s="3">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>4</v>
+      </c>
+      <c r="E6" s="3">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>4</v>
+      </c>
+      <c r="G6" s="3">
+        <v>2</v>
+      </c>
+      <c r="H6" s="4">
+        <v>4</v>
+      </c>
+      <c r="I6" s="4">
+        <v>2</v>
+      </c>
+      <c r="J6" s="3">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="K6" s="3">
+        <v>12</v>
+      </c>
+      <c r="L6" s="3">
         <v>6</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="J3" s="2" t="s">
+      <c r="M6" s="3">
+        <v>12</v>
+      </c>
+      <c r="N6" s="3">
         <v>6</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L3" s="2" t="s">
+      <c r="O6" s="3">
+        <v>12</v>
+      </c>
+      <c r="P6" s="3">
         <v>6</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="5">
-        <v>280</v>
-      </c>
-      <c r="D4" s="5">
-        <v>280</v>
-      </c>
-      <c r="E4" s="5">
-        <v>280</v>
-      </c>
-      <c r="F4" s="5">
-        <v>280</v>
-      </c>
-      <c r="G4" s="5">
-        <v>280</v>
-      </c>
-      <c r="H4" s="6">
-        <v>280</v>
-      </c>
-      <c r="I4" s="5">
-        <v>280</v>
-      </c>
-      <c r="J4" s="5">
-        <v>280</v>
-      </c>
-      <c r="K4" s="5">
-        <v>280</v>
-      </c>
-      <c r="L4" s="5">
-        <v>280</v>
-      </c>
-      <c r="M4" s="5">
-        <v>280</v>
-      </c>
-      <c r="N4" s="5">
-        <v>280</v>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3">
+        <v>277</v>
+      </c>
+      <c r="D7" s="3">
+        <v>275</v>
+      </c>
+      <c r="E7" s="3">
+        <v>277</v>
+      </c>
+      <c r="F7" s="3">
+        <v>275</v>
+      </c>
+      <c r="G7" s="3">
+        <v>277</v>
+      </c>
+      <c r="H7" s="3">
+        <v>275</v>
+      </c>
+      <c r="I7" s="3">
+        <v>277</v>
+      </c>
+      <c r="J7" s="3">
+        <v>273</v>
+      </c>
+      <c r="K7" s="3">
+        <v>267</v>
+      </c>
+      <c r="L7" s="3">
+        <v>273</v>
+      </c>
+      <c r="M7" s="3">
+        <v>267</v>
+      </c>
+      <c r="N7" s="3">
+        <v>273</v>
+      </c>
+      <c r="O7" s="3">
+        <v>267</v>
+      </c>
+      <c r="P7" s="3">
+        <v>273</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="5">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="D5" s="5">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="E5" s="5">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0.185</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0.105</v>
-      </c>
-      <c r="H5" s="6">
-        <v>0.114</v>
-      </c>
-      <c r="I5" s="5">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0.23499999999999999</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0.19</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="M5" s="5">
-        <v>7.1999999999999995E-2</v>
-      </c>
-      <c r="N5" s="5">
-        <v>0.19</v>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="20">
+        <v>-3.9E-2</v>
+      </c>
+      <c r="D8" s="20">
+        <v>-4.4900000000000002E-2</v>
+      </c>
+      <c r="E8" s="20">
+        <v>-8.6699999999999999E-2</v>
+      </c>
+      <c r="F8" s="20">
+        <v>-8.8700000000000001E-2</v>
+      </c>
+      <c r="G8" s="20">
+        <v>-4.8399999999999999E-2</v>
+      </c>
+      <c r="H8" s="12">
+        <v>-5.2499999999999998E-2</v>
+      </c>
+      <c r="I8" s="12">
+        <v>-0.129011186</v>
+      </c>
+      <c r="J8" s="20">
+        <v>-4.4999999999999998E-2</v>
+      </c>
+      <c r="K8" s="20">
+        <v>-0.11609999999999999</v>
+      </c>
+      <c r="L8" s="20">
+        <v>-9.1499999999999998E-2</v>
+      </c>
+      <c r="M8" s="20">
+        <v>-0.1328</v>
+      </c>
+      <c r="N8" s="20">
+        <v>-3.2500000000000001E-2</v>
+      </c>
+      <c r="O8" s="20">
+        <v>-9.1700000000000004E-2</v>
+      </c>
+      <c r="P8" s="20">
+        <v>-0.173925197</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="5">
-        <v>2</v>
-      </c>
-      <c r="D6" s="5">
-        <v>4</v>
-      </c>
-      <c r="E6" s="5">
-        <v>2</v>
-      </c>
-      <c r="F6" s="5">
-        <v>4</v>
-      </c>
-      <c r="G6" s="5">
-        <v>2</v>
-      </c>
-      <c r="H6" s="6">
-        <v>4</v>
-      </c>
-      <c r="I6" s="5">
-        <v>6</v>
-      </c>
-      <c r="J6" s="5">
-        <v>12</v>
-      </c>
-      <c r="K6" s="5">
-        <v>6</v>
-      </c>
-      <c r="L6" s="5">
-        <v>12</v>
-      </c>
-      <c r="M6" s="5">
-        <v>6</v>
-      </c>
-      <c r="N6" s="5">
-        <v>12</v>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="D9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="E9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="F9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="G9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="H9" s="12">
+        <v>2.4472</v>
+      </c>
+      <c r="I9" s="12">
+        <v>2.4471580309999998</v>
+      </c>
+      <c r="J9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="K9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="L9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="M9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="N9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="O9" s="20">
+        <v>2.4472</v>
+      </c>
+      <c r="P9" s="20">
+        <v>2.4471580309999998</v>
       </c>
     </row>
-    <row r="7" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="5">
-        <v>277</v>
-      </c>
-      <c r="D7" s="5">
-        <v>275</v>
-      </c>
-      <c r="E7" s="5">
-        <v>277</v>
-      </c>
-      <c r="F7" s="5">
-        <v>275</v>
-      </c>
-      <c r="G7" s="5">
-        <v>277</v>
-      </c>
-      <c r="H7" s="5">
-        <v>275</v>
-      </c>
-      <c r="I7" s="5">
-        <v>273</v>
-      </c>
-      <c r="J7" s="5">
-        <v>267</v>
-      </c>
-      <c r="K7" s="5">
-        <v>273</v>
-      </c>
-      <c r="L7" s="5">
-        <v>267</v>
-      </c>
-      <c r="M7" s="5">
-        <v>273</v>
-      </c>
-      <c r="N7" s="5">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7" t="s">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="8">
-        <v>-3.9E-2</v>
-      </c>
-      <c r="D8" s="8">
-        <v>-4.4900000000000002E-2</v>
-      </c>
-      <c r="E8" s="8">
-        <v>-8.6699999999999999E-2</v>
-      </c>
-      <c r="F8" s="8">
-        <v>-8.8700000000000001E-2</v>
-      </c>
-      <c r="G8" s="8">
-        <v>-4.8399999999999999E-2</v>
-      </c>
-      <c r="H8" s="9">
-        <v>-5.2499999999999998E-2</v>
-      </c>
-      <c r="I8" s="8">
-        <v>-4.4999999999999998E-2</v>
-      </c>
-      <c r="J8" s="8">
-        <v>-0.11609999999999999</v>
-      </c>
-      <c r="K8" s="8">
-        <v>-9.1499999999999998E-2</v>
-      </c>
-      <c r="L8" s="8">
-        <v>-0.1328</v>
-      </c>
-      <c r="M8" s="8">
-        <v>-3.2500000000000001E-2</v>
-      </c>
-      <c r="N8" s="8">
-        <v>-9.1700000000000004E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="D9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="E9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="F9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="G9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="H9" s="9">
-        <v>2.4472</v>
-      </c>
-      <c r="I9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="J9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="K9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="L9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="M9" s="8">
-        <v>2.4472</v>
-      </c>
-      <c r="N9" s="8">
-        <v>2.4472</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="10">
+      <c r="C10" s="13">
         <v>-6.0194000000000001</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="13">
         <v>-2.7759999999999998</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="13">
         <v>-19.386900000000001</v>
       </c>
-      <c r="F10" s="10">
+      <c r="F10" s="13">
         <v>-15.043699999999999</v>
       </c>
-      <c r="G10" s="10">
+      <c r="G10" s="13">
         <v>-8.6502999999999997</v>
       </c>
-      <c r="H10" s="10">
+      <c r="H10" s="13">
         <v>-4.9095000000000004</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="13">
+        <v>-31.228816080000001</v>
+      </c>
+      <c r="J10" s="13">
         <v>2.0718999999999999</v>
       </c>
-      <c r="J10" s="10">
+      <c r="K10" s="13">
         <v>-3.1524000000000001</v>
       </c>
-      <c r="K10" s="10">
+      <c r="L10" s="13">
         <v>-10.9452</v>
       </c>
-      <c r="L10" s="10">
+      <c r="M10" s="13">
         <v>-7.8311999999999999</v>
       </c>
-      <c r="M10" s="10">
+      <c r="N10" s="13">
         <v>5.5864000000000003</v>
       </c>
-      <c r="N10" s="10">
+      <c r="O10" s="13">
         <v>3.6865000000000001</v>
+      </c>
+      <c r="P10" s="13">
+        <v>-34.016107060000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="C1:H1"/>
-    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="J1:P1"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:F2"/>
+    <mergeCell ref="J2:K2"/>
+    <mergeCell ref="L2:M2"/>
     <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="N2:O2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>